<commit_message>
style: format code with Prettier
</commit_message>
<xml_diff>
--- a/DB/tracking.xlsx
+++ b/DB/tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\JavaScript_Note\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45A2A80C-5C8D-4C74-A842-D80DBF538DD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBE08C21-5AD4-4F27-9059-174C538527A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -78,7 +78,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -203,7 +203,7 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="7" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -736,10 +736,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{024DA12C-11CE-4CC1-B34A-E7E450722B61}">
-  <dimension ref="A2:B25"/>
+  <dimension ref="A2:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16:G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -864,7 +864,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
         <v>44877</v>
       </c>
@@ -872,45 +872,51 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="6">
         <v>44878</v>
       </c>
       <c r="B18">
         <v>6</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C18">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="6">
         <v>44879</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" s="4" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" s="4" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A20" s="6">
         <v>44880</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="6">
         <v>44881</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A22" s="6">
         <v>44882</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" s="6">
         <v>44883</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A24" s="6">
         <v>44884</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A25" s="6">
         <v>44885</v>
       </c>

</xml_diff>

<commit_message>
Format code with Prettier
</commit_message>
<xml_diff>
--- a/DB/tracking.xlsx
+++ b/DB/tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\JavaScript_Note\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45A2A80C-5C8D-4C74-A842-D80DBF538DD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBE08C21-5AD4-4F27-9059-174C538527A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -78,7 +78,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -203,7 +203,7 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="7" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -736,10 +736,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{024DA12C-11CE-4CC1-B34A-E7E450722B61}">
-  <dimension ref="A2:B25"/>
+  <dimension ref="A2:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16:G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -864,7 +864,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
         <v>44877</v>
       </c>
@@ -872,45 +872,51 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="6">
         <v>44878</v>
       </c>
       <c r="B18">
         <v>6</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C18">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="6">
         <v>44879</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" s="4" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" s="4" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A20" s="6">
         <v>44880</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="6">
         <v>44881</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A22" s="6">
         <v>44882</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" s="6">
         <v>44883</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A24" s="6">
         <v>44884</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A25" s="6">
         <v>44885</v>
       </c>

</xml_diff>